<commit_message>
Included an AES encryption for database protection and modified the config file accordingly
</commit_message>
<xml_diff>
--- a/clothing_store_data.xlsx
+++ b/clothing_store_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssu-my.sharepoint.com/personal/1mensd41_solent_ac_uk/Documents/SOLENT 2ND YEAR 24-25/ADVANCED DATABASE SYSTEMS(QHO541)/Clothing Store Database System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{32430041-F227-E342-ADF0-50699FC754B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{377A2E95-12AC-1C45-B200-7AB42ECC0A11}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{32430041-F227-E342-ADF0-50699FC754B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EB71FCD-55D7-4180-A014-640CCCA41096}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1580" windowWidth="28040" windowHeight="17260" xr2:uid="{A359667A-B457-C949-AEE0-E038B80A7A4B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A359667A-B457-C949-AEE0-E038B80A7A4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{5C34850F-4568-7F4E-BCF6-E5637EC8BE3F}" name="excel_data" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/kobxx/Downloads/excel_data.tsx">
+    <textPr sourceFile="/Users/kobxx/Downloads/excel_data.tsx">
       <textFields>
         <textField/>
       </textFields>
@@ -273,12 +273,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -627,11 +625,11 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -644,7 +642,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -658,7 +656,7 @@
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -672,7 +670,7 @@
       <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -686,7 +684,7 @@
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -700,7 +698,7 @@
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -714,7 +712,7 @@
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -732,7 +730,7 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -818,7 +816,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -868,11 +866,11 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -885,7 +883,7 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
@@ -902,7 +900,7 @@
       <c r="C2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <v>43845</v>
       </c>
       <c r="E2">
@@ -919,7 +917,7 @@
       <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>44256</v>
       </c>
       <c r="E3">
@@ -936,7 +934,7 @@
       <c r="C4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>44362</v>
       </c>
       <c r="E4">
@@ -953,7 +951,7 @@
       <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>44075</v>
       </c>
       <c r="E5">
@@ -970,7 +968,7 @@
       <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>43922</v>
       </c>
       <c r="E6">
@@ -991,9 +989,9 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9"/>
   <cols>
-    <col min="6" max="6" width="21" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1012,7 +1010,7 @@
       <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1032,7 +1030,7 @@
       <c r="E2">
         <v>38.979999999999997</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <v>45047.4375</v>
       </c>
     </row>
@@ -1052,7 +1050,7 @@
       <c r="E3">
         <v>79.989999999999995</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>45048.614583333336</v>
       </c>
     </row>
@@ -1072,7 +1070,7 @@
       <c r="E4">
         <v>49.99</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>45049.46875</v>
       </c>
     </row>
@@ -1092,7 +1090,7 @@
       <c r="E5">
         <v>129.99</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>45050.666666666664</v>
       </c>
     </row>
@@ -1112,7 +1110,7 @@
       <c r="E6">
         <v>179.98</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>45051.5625</v>
       </c>
     </row>

</xml_diff>